<commit_message>
Day3, working on the subtotal/groupby
</commit_message>
<xml_diff>
--- a/new_book.xlsx
+++ b/new_book.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,157 +436,168 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Budget Type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 1</t>
+          <t xml:space="preserve">Activity </t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 2</t>
+          <t>Clinical Study Number</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 3</t>
+          <t>Clinical Study Name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 4</t>
+          <t>Cost Type</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Budget 2021</t>
+          <t>Budget Q1 2021</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 6</t>
+          <t>Budget Q2 2021</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 7</t>
+          <t>Budget Q3 2021</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 8</t>
+          <t>Budget Q4 2021</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 9</t>
+          <t xml:space="preserve">  Budget FY 2021</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>April Exchange 2021</t>
+          <t>April Reforecast Q1 2021</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 11</t>
+          <t>April Reforecast Q2 2021</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 12</t>
+          <t>April Reforecast Q3 2021</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 13</t>
+          <t>April Reforecast Q4 2021</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 14</t>
+          <t xml:space="preserve">  April Reforecast FY 2021</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Actuals 2021</t>
+          <t>Actuals Q1 2021</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 16</t>
+          <t>Actuals Q2 2021</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 17</t>
+          <t>Actuals Q3 2021</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 18</t>
+          <t>Actuals Q4 2021</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 19</t>
+          <t xml:space="preserve">  Actuals FY 2021</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Variance Actuals vs Budget 2021</t>
+          <t>Variance Q1 2021</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 21</t>
+          <t>Variance Q2 2021</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 22</t>
+          <t>Variance Q3 2021</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 23</t>
+          <t>Variance Q4 2021</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 24</t>
+          <t xml:space="preserve">  Variance FY 2021</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Variance Actuals vs April Exchange 2021</t>
+          <t>Variance Q1 2021.1</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 26</t>
+          <t>Variance Q2 2021.1</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 27</t>
+          <t>Variance Q3 2021.1</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 28</t>
+          <t>Variance Q4 2021.1</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 29</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 30</t>
+          <t xml:space="preserve">  Variance FY 2021.1</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr"/>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Budget FY recal</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>April Reforecast FY recal</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Actuals FY recal</t>
         </is>
       </c>
     </row>
@@ -596,155 +607,112 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Budget Type</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Activity </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Clinical Study Number</t>
-        </is>
+          <t>Clinical</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>54321</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Clinical Study Name</t>
+          <t>Study 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cost Type</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Budget Q1 2021</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Budget Q2 2021</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Budget Q3 2021</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Budget Q4 2021</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Budget FY 2021</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>April Reforecast Q1 2021</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>April Reforecast Q2 2021</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>April Reforecast Q3 2021</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>April Reforecast Q4 2021</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  April Reforecast FY 2021</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Actuals Q1 2021</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Actuals Q2 2021</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Actuals Q3 2021</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Actuals Q4 2021</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Actuals FY 2021</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Variance Q1 2021</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Variance Q2 2021</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Variance Q3 2021</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>Variance Q4 2021</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Variance FY 2021</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>Variance Q1 2021</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>Variance Q2 2021</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>Variance Q3 2021</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>Variance Q4 2021</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Variance FY 2021</t>
-        </is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>145.8396011909514</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.618317326377889</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>150.4579185173292</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>100.1749402002227</v>
+      </c>
+      <c r="R2" t="n">
+        <v>56.88785212267903</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>157.0627923229017</v>
+      </c>
+      <c r="V2" t="n">
+        <v>100.1749402002227</v>
+      </c>
+      <c r="W2" t="n">
+        <v>56.88785212267903</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>157.0627923229017</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>-45.66466099072863</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>52.26953479630114</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>6.60487380557251</v>
       </c>
       <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -760,59 +728,69 @@
           <t>Clinical</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>630CV01C4931 - Pcsk9.CV.HC.Clin.4931-1532</t>
-        </is>
+      <c r="D3" t="n">
+        <v>54321</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R727-CL-1532 Neuroccog Study</t>
+          <t>Study 1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>145.8396011909514</v>
+        <v>605.9270070000002</v>
       </c>
       <c r="M3" t="n">
-        <v>4.618317326377889</v>
+        <v>173.2898607117995</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>46.93815700000022</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>150.4579185173292</v>
+        <v>826.1550247118</v>
       </c>
       <c r="Q3" t="n">
-        <v>100.1749402002227</v>
+        <v>163.38793</v>
       </c>
       <c r="R3" t="n">
-        <v>56.88785212267903</v>
-      </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+        <v>6702.08531</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
       <c r="U3" t="n">
-        <v>157.0627923229017</v>
+        <v>6865.47324</v>
       </c>
       <c r="V3" t="n">
-        <v>100.1749402002227</v>
+        <v>263.5628702002227</v>
       </c>
       <c r="W3" t="n">
-        <v>56.88785212267903</v>
+        <v>6702.08531</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -821,24 +799,33 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>157.0627923229017</v>
+        <v>6865.47324</v>
       </c>
       <c r="AA3" t="n">
-        <v>-45.66466099072863</v>
+        <v>-442.5390770000002</v>
       </c>
       <c r="AB3" t="n">
-        <v>52.26953479630114</v>
+        <v>6528.795449288201</v>
       </c>
       <c r="AC3" t="n">
-        <v>0</v>
+        <v>-46.93815700000022</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>6.60487380557251</v>
+        <v>6039.3182152882</v>
       </c>
       <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -856,31 +843,35 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>630CV01C4931 - Pcsk9.CV.HC.Clin.4931-1532</t>
+          <t>54321 Total</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R727-CL-1532 Neuroccog Study</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+          <t>Study 1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>605.9270070000002</v>
+        <v>751.7666081909516</v>
       </c>
       <c r="M4" t="n">
-        <v>173.2898607117995</v>
+        <v>177.9081780381773</v>
       </c>
       <c r="N4" t="n">
         <v>46.93815700000022</v>
@@ -889,24 +880,28 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>826.1550247118</v>
+        <v>976.6129432291293</v>
       </c>
       <c r="Q4" t="n">
-        <v>163.38793</v>
+        <v>263.5628702002227</v>
       </c>
       <c r="R4" t="n">
-        <v>6702.08531</v>
-      </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+        <v>6758.973162122679</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
       <c r="U4" t="n">
-        <v>6865.47324</v>
+        <v>7022.536032322902</v>
       </c>
       <c r="V4" t="n">
         <v>263.5628702002227</v>
       </c>
       <c r="W4" t="n">
-        <v>6702.08531</v>
+        <v>6758.973162122679</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -915,13 +910,13 @@
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>6865.47324</v>
+        <v>7022.536032322902</v>
       </c>
       <c r="AA4" t="n">
-        <v>-442.5390770000002</v>
+        <v>-488.2037379907289</v>
       </c>
       <c r="AB4" t="n">
-        <v>6528.795449288201</v>
+        <v>6581.064984084502</v>
       </c>
       <c r="AC4" t="n">
         <v>-46.93815700000022</v>
@@ -930,12 +925,17 @@
         <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>6039.3182152882</v>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>CRO close out costs forecasted in Apr BOD did not include Accounting release of pre-paid expenses to account for competitive enrollment. Close out costs were re-evaluated and updated in the Jun BOD (forecast not shared with Sanofi)</t>
-        </is>
+        <v>6045.923089093773</v>
+      </c>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>-2.273736754432321e-13</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>-9.094947017729282e-13</v>
       </c>
     </row>
     <row r="5">
@@ -952,17 +952,19 @@
           <t>Clinical</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>630CV01C4931 - Pcsk9.CV.HC.Clin.4931-1532 Total</t>
-        </is>
+      <c r="D5" t="n">
+        <v>65432</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R727-CL-1532 Neuroccog Study</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>Study 2</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
@@ -979,25 +981,25 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>751.7666081909516</v>
+        <v>164.147828713069</v>
       </c>
       <c r="M5" t="n">
-        <v>177.9081780381773</v>
+        <v>127.1387018473341</v>
       </c>
       <c r="N5" t="n">
-        <v>46.93815700000022</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>976.6129432291293</v>
+        <v>291.2865305604031</v>
       </c>
       <c r="Q5" t="n">
-        <v>263.5628702002227</v>
+        <v>137.4580618906389</v>
       </c>
       <c r="R5" t="n">
-        <v>6758.973162122679</v>
+        <v>42.60160124201722</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -1006,13 +1008,13 @@
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>7022.536032322902</v>
+        <v>180.0596631326561</v>
       </c>
       <c r="V5" t="n">
-        <v>263.5628702002227</v>
+        <v>137.4580618906389</v>
       </c>
       <c r="W5" t="n">
-        <v>6758.973162122679</v>
+        <v>42.60160124201722</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -1021,24 +1023,33 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>7022.536032322902</v>
+        <v>180.0596631326561</v>
       </c>
       <c r="AA5" t="n">
-        <v>-488.2037379907289</v>
+        <v>-26.68976682243016</v>
       </c>
       <c r="AB5" t="n">
-        <v>6581.064984084502</v>
+        <v>-84.53710060531685</v>
       </c>
       <c r="AC5" t="n">
-        <v>-46.93815700000022</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>6045.923089093773</v>
+        <v>-111.226867427747</v>
       </c>
       <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1054,59 +1065,69 @@
           <t>Clinical</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">630CV01C4932- R727-CL-1609 Neurocog (PASS) </t>
-        </is>
+      <c r="D6" t="n">
+        <v>65432</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">R727-CL-1609 Neurocog (PASS) </t>
+          <t>Study 2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>164.147828713069</v>
+        <v>38.41416</v>
       </c>
       <c r="M6" t="n">
-        <v>127.1387018473341</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1873.658000284128</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>291.2865305604031</v>
+        <v>1912.072160284128</v>
       </c>
       <c r="Q6" t="n">
-        <v>137.4580618906389</v>
+        <v>67.46408000000001</v>
       </c>
       <c r="R6" t="n">
-        <v>42.60160124201722</v>
-      </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
+        <v>91.08320000000001</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
       <c r="U6" t="n">
-        <v>180.0596631326561</v>
+        <v>158.54728</v>
       </c>
       <c r="V6" t="n">
-        <v>137.4580618906389</v>
+        <v>67.46408000000001</v>
       </c>
       <c r="W6" t="n">
-        <v>42.60160124201722</v>
+        <v>91.08320000000001</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -1115,24 +1136,33 @@
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>180.0596631326561</v>
+        <v>158.54728</v>
       </c>
       <c r="AA6" t="n">
-        <v>-26.68976682243016</v>
+        <v>29.04992000000001</v>
       </c>
       <c r="AB6" t="n">
-        <v>-84.53710060531685</v>
+        <v>91.08320000000001</v>
       </c>
       <c r="AC6" t="n">
-        <v>0</v>
+        <v>-1873.658000284128</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>-111.226867427747</v>
+        <v>-1753.524880284128</v>
       </c>
       <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1150,31 +1180,35 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">630CV01C4932- R727-CL-1609 Neurocog (PASS) </t>
+          <t>65432 Total</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">R727-CL-1609 Neurocog (PASS) </t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+          <t>Study 2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>38.41416</v>
+        <v>202.561988713069</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>127.1387018473341</v>
       </c>
       <c r="N7" t="n">
         <v>1873.658000284128</v>
@@ -1183,24 +1217,28 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>1912.072160284128</v>
+        <v>2203.358690844531</v>
       </c>
       <c r="Q7" t="n">
-        <v>67.46408000000001</v>
+        <v>204.9221418906389</v>
       </c>
       <c r="R7" t="n">
-        <v>91.08320000000001</v>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
+        <v>133.6848012420172</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
       <c r="U7" t="n">
-        <v>158.54728</v>
+        <v>338.6069431326561</v>
       </c>
       <c r="V7" t="n">
-        <v>67.46408000000001</v>
+        <v>204.9221418906389</v>
       </c>
       <c r="W7" t="n">
-        <v>91.08320000000001</v>
+        <v>133.6848012420172</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1209,13 +1247,13 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>158.54728</v>
+        <v>338.6069431326561</v>
       </c>
       <c r="AA7" t="n">
-        <v>29.04992000000001</v>
+        <v>2.360153177569856</v>
       </c>
       <c r="AB7" t="n">
-        <v>91.08320000000001</v>
+        <v>6.546099394683139</v>
       </c>
       <c r="AC7" t="n">
         <v>-1873.658000284128</v>
@@ -1224,9 +1262,18 @@
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>-1753.524880284128</v>
+        <v>-1864.751747711875</v>
       </c>
       <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1242,17 +1289,19 @@
           <t>Clinical</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>630CV01C4932- R727-CL-1609 Neurocog (PASS) Total</t>
-        </is>
+      <c r="D8" t="n">
+        <v>87653</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">R727-CL-1609 Neurocog (PASS) </t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Study 3</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
@@ -1269,25 +1318,25 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>202.561988713069</v>
+        <v>463.2701079898713</v>
       </c>
       <c r="M8" t="n">
-        <v>127.1387018473341</v>
+        <v>299.5683897499085</v>
       </c>
       <c r="N8" t="n">
-        <v>1873.658000284128</v>
+        <v>305.7192174493194</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>285.6510791489375</v>
       </c>
       <c r="P8" t="n">
-        <v>2203.358690844531</v>
+        <v>1354.208794338037</v>
       </c>
       <c r="Q8" t="n">
-        <v>204.9221418906389</v>
+        <v>530.702483591282</v>
       </c>
       <c r="R8" t="n">
-        <v>133.6848012420172</v>
+        <v>554.6238013340608</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1296,13 +1345,13 @@
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>338.6069431326561</v>
+        <v>1085.326284925343</v>
       </c>
       <c r="V8" t="n">
-        <v>204.9221418906389</v>
+        <v>530.702483591282</v>
       </c>
       <c r="W8" t="n">
-        <v>133.6848012420172</v>
+        <v>554.6238013340608</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1311,24 +1360,33 @@
         <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>338.6069431326561</v>
+        <v>1085.326284925343</v>
       </c>
       <c r="AA8" t="n">
-        <v>2.360153177569856</v>
+        <v>67.43237560141063</v>
       </c>
       <c r="AB8" t="n">
-        <v>6.546099394683139</v>
+        <v>255.0554115841522</v>
       </c>
       <c r="AC8" t="n">
-        <v>-1873.658000284128</v>
+        <v>-305.7192174493194</v>
       </c>
       <c r="AD8" t="n">
-        <v>0</v>
+        <v>-285.6510791489375</v>
       </c>
       <c r="AE8" t="n">
-        <v>-1864.751747711875</v>
+        <v>-268.8825094126939</v>
       </c>
       <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1346,23 +1404,27 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
+          <t>87653 Total</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+          <t>Study 3</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
@@ -1387,8 +1449,12 @@
       <c r="R9" t="n">
         <v>554.6238013340608</v>
       </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
       <c r="U9" t="n">
         <v>1085.326284925343</v>
       </c>
@@ -1423,6 +1489,15 @@
         <v>-268.8825094126939</v>
       </c>
       <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1435,17 +1510,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Clinical</t>
+          <t>Clinical Total</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
+          <t>87653 Total</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
+          <t>Study 3</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -1465,25 +1540,25 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>463.2701079898713</v>
+        <v>1417.598704893892</v>
       </c>
       <c r="M10" t="n">
-        <v>299.5683897499085</v>
+        <v>604.61526963542</v>
       </c>
       <c r="N10" t="n">
-        <v>305.7192174493194</v>
+        <v>2226.315374733448</v>
       </c>
       <c r="O10" t="n">
         <v>285.6510791489375</v>
       </c>
       <c r="P10" t="n">
-        <v>1354.208794338037</v>
+        <v>4534.180428411697</v>
       </c>
       <c r="Q10" t="n">
-        <v>530.702483591282</v>
+        <v>999.1874956821435</v>
       </c>
       <c r="R10" t="n">
-        <v>554.6238013340608</v>
+        <v>7447.281764698757</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1492,13 +1567,13 @@
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>1085.326284925343</v>
+        <v>8446.469260380902</v>
       </c>
       <c r="V10" t="n">
-        <v>530.702483591282</v>
+        <v>999.1874956821435</v>
       </c>
       <c r="W10" t="n">
-        <v>554.6238013340608</v>
+        <v>7447.281764698757</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1507,24 +1582,33 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>1085.326284925343</v>
+        <v>8446.469260380902</v>
       </c>
       <c r="AA10" t="n">
-        <v>67.43237560141063</v>
+        <v>-418.4112092117485</v>
       </c>
       <c r="AB10" t="n">
-        <v>255.0554115841522</v>
+        <v>6842.666495063337</v>
       </c>
       <c r="AC10" t="n">
-        <v>-305.7192174493194</v>
+        <v>-2226.315374733448</v>
       </c>
       <c r="AD10" t="n">
         <v>-285.6510791489375</v>
       </c>
       <c r="AE10" t="n">
-        <v>-268.8825094126939</v>
+        <v>3912.288831969205</v>
       </c>
       <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>-1.818989403545856e-12</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1532,7 +1616,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Development Total</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1542,12 +1626,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
+          <t>87653 Total</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
+          <t>Study 3</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -1627,6 +1711,15 @@
         <v>3912.288831969205</v>
       </c>
       <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>-1.818989403545856e-12</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1634,7 +1727,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Development Total</t>
+          <t>Grand Total</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1644,12 +1737,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
+          <t>87653 Total</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
+          <t>Study 3</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -1729,31 +1822,26 @@
         <v>3912.288831969205</v>
       </c>
       <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>-1.818989403545856e-12</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Grand Total</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
-        </is>
-      </c>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>GrandTotal55</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>0</v>
@@ -1761,282 +1849,33 @@
       <c r="H13" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1417.598704893892</v>
-      </c>
-      <c r="M13" t="n">
-        <v>604.61526963542</v>
-      </c>
-      <c r="N13" t="n">
-        <v>2226.315374733448</v>
-      </c>
-      <c r="O13" t="n">
-        <v>285.6510791489375</v>
-      </c>
-      <c r="P13" t="n">
-        <v>4534.180428411697</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>999.1874956821435</v>
-      </c>
-      <c r="R13" t="n">
-        <v>7447.281764698757</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0</v>
-      </c>
-      <c r="U13" t="n">
-        <v>8446.469260380902</v>
-      </c>
-      <c r="V13" t="n">
-        <v>999.1874956821435</v>
-      </c>
-      <c r="W13" t="n">
-        <v>7447.281764698757</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>8446.469260380902</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>-418.4112092117485</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>6842.666495063337</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>-2226.315374733448</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>-285.6510791489375</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>3912.288831969205</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Grand Total</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Grand Total</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Grand Total</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>7447281.764698757</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen Total</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>630GE00G0000 - Pcsk9.Other.Gen.Gen.Gen</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Day6- row sum function works, need to work on the col sum function and adding the result in excel
</commit_message>
<xml_diff>
--- a/new_book.xlsx
+++ b/new_book.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,157 +434,150 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Budget Type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Activity </t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Clinical Study Number</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Clinical Study Name</t>
+          <t>Unnamed: 3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Cost Type</t>
+          <t>Unnamed: 4</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Budget Q1 2021</t>
+          <t>Budget 2021</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Budget Q2 2021</t>
+          <t>Unnamed: 6</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Budget Q3 2021</t>
+          <t>Unnamed: 7</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Budget Q4 2021</t>
+          <t>Unnamed: 8</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Budget FY 2021</t>
+          <t>Unnamed: 9</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>April Reforecast Q1 2021</t>
+          <t>April Exchange 2021</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>April Reforecast Q2 2021</t>
+          <t>Unnamed: 11</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>April Reforecast Q3 2021</t>
+          <t>Unnamed: 12</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>April Reforecast Q4 2021</t>
+          <t>Unnamed: 13</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">  April Reforecast FY 2021</t>
+          <t>Unnamed: 14</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Actuals Q1 2021</t>
+          <t>Actuals 2021</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Actuals Q2 2021</t>
+          <t>Unnamed: 16</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Actuals Q3 2021</t>
+          <t>Unnamed: 17</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Actuals Q4 2021</t>
+          <t>Unnamed: 18</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Actuals FY 2021</t>
+          <t>Unnamed: 19</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q1 2021</t>
+          <t>Variance Actuals vs Budget 2021</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q2 2021</t>
+          <t>Unnamed: 21</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q3 2021</t>
+          <t>Unnamed: 22</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q4 2021</t>
+          <t>Unnamed: 23</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Variance FY 2021</t>
+          <t>Unnamed: 24</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q1 2021.1</t>
+          <t>Variance Actuals vs April Exchange 2021</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q2 2021.1</t>
+          <t>Unnamed: 26</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q3 2021.1</t>
+          <t>Unnamed: 27</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Variance Q4 2021.1</t>
+          <t>Unnamed: 28</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Variance FY 2021.1</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr"/>
+          <t>Unnamed: 29</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -592,91 +585,154 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Budget Type</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Clinical</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>54321</v>
+          <t xml:space="preserve">Activity </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Clinical Study Number</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Study 1</t>
+          <t>Clinical Study Name</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>145.8396011909514</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.618317326377889</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>150.4579185173292</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>100.1749402002227</v>
-      </c>
-      <c r="R2" t="n">
-        <v>56.88785212267903</v>
-      </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>157.0627923229017</v>
-      </c>
-      <c r="V2" t="n">
-        <v>100.1749402002227</v>
-      </c>
-      <c r="W2" t="n">
-        <v>56.88785212267903</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>157.0627923229017</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>-45.66466099072863</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>52.26953479630114</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>6.60487380557251</v>
-      </c>
-      <c r="AF2" t="inlineStr"/>
+          <t>Cost Type</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Budget Q1 2021</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Budget Q2 2021</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Budget Q3 2021</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Budget Q4 2021</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Budget FY 2021</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>April Reforecast Q1 2021</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>April Reforecast Q2 2021</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>April Reforecast Q3 2021</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>April Reforecast Q4 2021</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  April Reforecast FY 2021</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Actuals Q1 2021</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Actuals Q2 2021</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Actuals Q3 2021</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Actuals Q4 2021</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Actuals FY 2021</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Variance Q1 2021</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Variance Q2 2021</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Variance Q3 2021</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Variance Q4 2021</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Variance FY 2021</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Variance Q1 2021</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Variance Q2 2021</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Variance Q3 2021</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Variance Q4 2021</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Variance FY 2021</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -702,7 +758,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -713,36 +769,36 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>605.9270070000002</v>
+        <v>145.8396011909514</v>
       </c>
       <c r="M3" t="n">
-        <v>173.2898607117995</v>
+        <v>4.618317326377889</v>
       </c>
       <c r="N3" t="n">
-        <v>46.93815700000022</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>826.1550247118</v>
+        <v>150.4579185173292</v>
       </c>
       <c r="Q3" t="n">
-        <v>163.38793</v>
+        <v>100.1749402002227</v>
       </c>
       <c r="R3" t="n">
-        <v>6702.08531</v>
+        <v>56.88785212267903</v>
       </c>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>6865.47324</v>
+        <v>157.0627923229017</v>
       </c>
       <c r="V3" t="n">
-        <v>263.5628702002227</v>
+        <v>100.1749402002227</v>
       </c>
       <c r="W3" t="n">
-        <v>6702.08531</v>
+        <v>56.88785212267903</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -751,70 +807,51 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>6865.47324</v>
+        <v>157.0627923229017</v>
       </c>
       <c r="AA3" t="n">
-        <v>-442.5390770000002</v>
+        <v>-45.66466099072863</v>
       </c>
       <c r="AB3" t="n">
-        <v>6528.795449288201</v>
+        <v>52.26953479630114</v>
       </c>
       <c r="AC3" t="n">
-        <v>-46.93815700000022</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>6039.3182152882</v>
-      </c>
-      <c r="AF3" t="inlineStr"/>
+        <v>6.60487380557251</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Clinical</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>54321 Total</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Study 1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>54321</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>751.7666081909516</v>
+        <v>605.9270070000002</v>
       </c>
       <c r="M4" t="n">
-        <v>177.9081780381773</v>
+        <v>173.2898607117995</v>
       </c>
       <c r="N4" t="n">
         <v>46.93815700000022</v>
@@ -823,28 +860,24 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>976.6129432291293</v>
+        <v>826.1550247118</v>
       </c>
       <c r="Q4" t="n">
-        <v>263.5628702002227</v>
+        <v>163.38793</v>
       </c>
       <c r="R4" t="n">
-        <v>6758.973162122679</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
+        <v>6702.08531</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
-        <v>7022.536032322902</v>
+        <v>6865.47324</v>
       </c>
       <c r="V4" t="n">
         <v>263.5628702002227</v>
       </c>
       <c r="W4" t="n">
-        <v>6758.973162122679</v>
+        <v>6702.08531</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -853,13 +886,13 @@
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>7022.536032322902</v>
+        <v>6865.47324</v>
       </c>
       <c r="AA4" t="n">
-        <v>-488.2037379907289</v>
+        <v>-442.5390770000002</v>
       </c>
       <c r="AB4" t="n">
-        <v>6581.064984084502</v>
+        <v>6528.795449288201</v>
       </c>
       <c r="AC4" t="n">
         <v>-46.93815700000022</v>
@@ -868,75 +901,72 @@
         <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>6045.923089093773</v>
-      </c>
-      <c r="AF4" t="inlineStr"/>
+        <v>6039.3182152882</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Clinical</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>65432</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Study 2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>54321 Total</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>164.147828713069</v>
+        <v>751.7666081909516</v>
       </c>
       <c r="M5" t="n">
-        <v>127.1387018473341</v>
+        <v>177.9081780381773</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>46.93815700000022</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>291.2865305604031</v>
+        <v>976.6129432291293</v>
       </c>
       <c r="Q5" t="n">
-        <v>137.4580618906389</v>
+        <v>263.5628702002227</v>
       </c>
       <c r="R5" t="n">
-        <v>42.60160124201722</v>
-      </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
+        <v>6758.973162122679</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
       <c r="U5" t="n">
-        <v>180.0596631326561</v>
+        <v>7022.536032322902</v>
       </c>
       <c r="V5" t="n">
-        <v>137.4580618906389</v>
+        <v>263.5628702002227</v>
       </c>
       <c r="W5" t="n">
-        <v>42.60160124201722</v>
+        <v>6758.973162122679</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -945,39 +975,30 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>180.0596631326561</v>
+        <v>7022.536032322902</v>
       </c>
       <c r="AA5" t="n">
-        <v>-26.68976682243016</v>
+        <v>-488.2037379907289</v>
       </c>
       <c r="AB5" t="n">
-        <v>-84.53710060531685</v>
+        <v>6581.064984084502</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>-46.93815700000022</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>-111.226867427747</v>
-      </c>
-      <c r="AF5" t="inlineStr"/>
+        <v>6045.923089093773</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Clinical</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
         <v>65432</v>
       </c>
@@ -988,7 +1009,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -999,36 +1020,36 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>38.41416</v>
+        <v>164.147828713069</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>127.1387018473341</v>
       </c>
       <c r="N6" t="n">
-        <v>1873.658000284128</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>1912.072160284128</v>
+        <v>291.2865305604031</v>
       </c>
       <c r="Q6" t="n">
-        <v>67.46408000000001</v>
+        <v>137.4580618906389</v>
       </c>
       <c r="R6" t="n">
-        <v>91.08320000000001</v>
+        <v>42.60160124201722</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
-        <v>158.54728</v>
+        <v>180.0596631326561</v>
       </c>
       <c r="V6" t="n">
-        <v>67.46408000000001</v>
+        <v>137.4580618906389</v>
       </c>
       <c r="W6" t="n">
-        <v>91.08320000000001</v>
+        <v>42.60160124201722</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -1037,70 +1058,49 @@
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>158.54728</v>
+        <v>180.0596631326561</v>
       </c>
       <c r="AA6" t="n">
-        <v>29.04992000000001</v>
+        <v>-26.68976682243016</v>
       </c>
       <c r="AB6" t="n">
-        <v>91.08320000000001</v>
+        <v>-84.53710060531685</v>
       </c>
       <c r="AC6" t="n">
-        <v>-1873.658000284128</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>-1753.524880284128</v>
-      </c>
-      <c r="AF6" t="inlineStr"/>
+        <v>-111.226867427747</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Clinical</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>65432 Total</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Study 2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>202.561988713069</v>
+        <v>38.41416</v>
       </c>
       <c r="M7" t="n">
-        <v>127.1387018473341</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>1873.658000284128</v>
@@ -1109,28 +1109,24 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>2203.358690844531</v>
+        <v>1912.072160284128</v>
       </c>
       <c r="Q7" t="n">
-        <v>204.9221418906389</v>
+        <v>67.46408000000001</v>
       </c>
       <c r="R7" t="n">
-        <v>133.6848012420172</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
+        <v>91.08320000000001</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="n">
-        <v>338.6069431326561</v>
+        <v>158.54728</v>
       </c>
       <c r="V7" t="n">
-        <v>204.9221418906389</v>
+        <v>67.46408000000001</v>
       </c>
       <c r="W7" t="n">
-        <v>133.6848012420172</v>
+        <v>91.08320000000001</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1139,13 +1135,13 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>338.6069431326561</v>
+        <v>158.54728</v>
       </c>
       <c r="AA7" t="n">
-        <v>2.360153177569856</v>
+        <v>29.04992000000001</v>
       </c>
       <c r="AB7" t="n">
-        <v>6.546099394683139</v>
+        <v>91.08320000000001</v>
       </c>
       <c r="AC7" t="n">
         <v>-1873.658000284128</v>
@@ -1154,75 +1150,72 @@
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>-1864.751747711875</v>
-      </c>
-      <c r="AF7" t="inlineStr"/>
+        <v>-1753.524880284128</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Clinical</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>87653</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Study 3</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>65432 Total</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>463.2701079898713</v>
+        <v>202.561988713069</v>
       </c>
       <c r="M8" t="n">
-        <v>299.5683897499085</v>
+        <v>127.1387018473341</v>
       </c>
       <c r="N8" t="n">
-        <v>305.7192174493194</v>
+        <v>1873.658000284128</v>
       </c>
       <c r="O8" t="n">
-        <v>285.6510791489375</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>1354.208794338037</v>
+        <v>2203.358690844531</v>
       </c>
       <c r="Q8" t="n">
-        <v>530.702483591282</v>
+        <v>204.9221418906389</v>
       </c>
       <c r="R8" t="n">
-        <v>554.6238013340608</v>
-      </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
+        <v>133.6848012420172</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
       <c r="U8" t="n">
-        <v>1085.326284925343</v>
+        <v>338.6069431326561</v>
       </c>
       <c r="V8" t="n">
-        <v>530.702483591282</v>
+        <v>204.9221418906389</v>
       </c>
       <c r="W8" t="n">
-        <v>554.6238013340608</v>
+        <v>133.6848012420172</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1231,62 +1224,47 @@
         <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>1085.326284925343</v>
+        <v>338.6069431326561</v>
       </c>
       <c r="AA8" t="n">
-        <v>67.43237560141063</v>
+        <v>2.360153177569856</v>
       </c>
       <c r="AB8" t="n">
-        <v>255.0554115841522</v>
+        <v>6.546099394683139</v>
       </c>
       <c r="AC8" t="n">
-        <v>-305.7192174493194</v>
+        <v>-1873.658000284128</v>
       </c>
       <c r="AD8" t="n">
-        <v>-285.6510791489375</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>-268.8825094126939</v>
-      </c>
-      <c r="AF8" t="inlineStr"/>
+        <v>-1864.751747711875</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Clinical</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>87653 Total</t>
-        </is>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>87653</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>Study 3</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
         <v>0</v>
       </c>
@@ -1311,12 +1289,8 @@
       <c r="R9" t="n">
         <v>554.6238013340608</v>
       </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0</v>
-      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="n">
         <v>1085.326284925343</v>
       </c>
@@ -1350,32 +1324,19 @@
       <c r="AE9" t="n">
         <v>-268.8825094126939</v>
       </c>
-      <c r="AF9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>87653 Total</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Study 3</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>0</v>
@@ -1393,25 +1354,25 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>1417.598704893892</v>
+        <v>463.2701079898713</v>
       </c>
       <c r="M10" t="n">
-        <v>604.61526963542</v>
+        <v>299.5683897499085</v>
       </c>
       <c r="N10" t="n">
-        <v>2226.315374733448</v>
+        <v>305.7192174493194</v>
       </c>
       <c r="O10" t="n">
         <v>285.6510791489375</v>
       </c>
       <c r="P10" t="n">
-        <v>4534.180428411697</v>
+        <v>1354.208794338037</v>
       </c>
       <c r="Q10" t="n">
-        <v>999.1874956821435</v>
+        <v>530.702483591282</v>
       </c>
       <c r="R10" t="n">
-        <v>7447.281764698757</v>
+        <v>554.6238013340608</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1420,13 +1381,13 @@
         <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>8446.469260380902</v>
+        <v>1085.326284925343</v>
       </c>
       <c r="V10" t="n">
-        <v>999.1874956821435</v>
+        <v>530.702483591282</v>
       </c>
       <c r="W10" t="n">
-        <v>7447.281764698757</v>
+        <v>554.6238013340608</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1435,49 +1396,36 @@
         <v>0</v>
       </c>
       <c r="Z10" t="n">
-        <v>8446.469260380902</v>
+        <v>1085.326284925343</v>
       </c>
       <c r="AA10" t="n">
-        <v>-418.4112092117485</v>
+        <v>67.43237560141063</v>
       </c>
       <c r="AB10" t="n">
-        <v>6842.666495063337</v>
+        <v>255.0554115841522</v>
       </c>
       <c r="AC10" t="n">
-        <v>-2226.315374733448</v>
+        <v>-305.7192174493194</v>
       </c>
       <c r="AD10" t="n">
         <v>-285.6510791489375</v>
       </c>
       <c r="AE10" t="n">
-        <v>3912.288831969205</v>
-      </c>
-      <c r="AF10" t="inlineStr"/>
+        <v>-268.8825094126939</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Development Total</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>Clinical Total</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>87653 Total</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Study 3</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>0</v>
@@ -1554,7 +1502,6 @@
       <c r="AE11" t="n">
         <v>3912.288831969205</v>
       </c>
-      <c r="AF11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1562,24 +1509,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Grand Total</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Clinical Total</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>87653 Total</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Study 3</t>
-        </is>
-      </c>
+          <t>Development Total</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>0</v>
@@ -1656,15 +1591,16 @@
       <c r="AE12" t="n">
         <v>3912.288831969205</v>
       </c>
-      <c r="AF12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>GrandTotal</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Grand Total</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
@@ -1685,25 +1621,25 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>7087.993524469461</v>
+        <v>1417.598704893892</v>
       </c>
       <c r="M13" t="n">
-        <v>3023.0763481771</v>
+        <v>604.61526963542</v>
       </c>
       <c r="N13" t="n">
-        <v>11131.57687366724</v>
+        <v>2226.315374733448</v>
       </c>
       <c r="O13" t="n">
-        <v>1428.255395744688</v>
+        <v>285.6510791489375</v>
       </c>
       <c r="P13" t="n">
-        <v>22670.90214205848</v>
+        <v>4534.180428411697</v>
       </c>
       <c r="Q13" t="n">
-        <v>4995.937478410718</v>
+        <v>999.1874956821435</v>
       </c>
       <c r="R13" t="n">
-        <v>37236.40882349378</v>
+        <v>7447.281764698757</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -1712,19 +1648,38 @@
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>42232.34630190451</v>
-      </c>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
+        <v>8446.469260380902</v>
+      </c>
+      <c r="V13" t="n">
+        <v>999.1874956821435</v>
+      </c>
+      <c r="W13" t="n">
+        <v>7447.281764698757</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>8446.469260380902</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>-418.4112092117485</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>6842.666495063337</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>-2226.315374733448</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>-285.6510791489375</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>3912.288831969205</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Day7- completed all the major parts, left with column subtract operation and group by labels on the bottom of the page
</commit_message>
<xml_diff>
--- a/new_book.xlsx
+++ b/new_book.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AI15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,6 +578,22 @@
           <t>Unnamed: 29</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr"/>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>budget_recal</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>april_reforecast_recal</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>actuals_recal</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -731,6 +747,22 @@
       <c r="AE2" t="inlineStr">
         <is>
           <t xml:space="preserve">  Variance FY 2021</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>budget_recal</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>april_reforecast_recal</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>actuals_recal</t>
         </is>
       </c>
     </row>
@@ -761,10 +793,18 @@
           <t>A</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
@@ -789,8 +829,12 @@
       <c r="R3" t="n">
         <v>56.88785212267903</v>
       </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
       <c r="U3" t="n">
         <v>157.0627923229017</v>
       </c>
@@ -823,27 +867,57 @@
       </c>
       <c r="AE3" t="n">
         <v>6.60487380557251</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>150.4579185173292</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>157.0627923229017</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
       <c r="D4" t="n">
         <v>54321</v>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Study 1</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
@@ -868,8 +942,12 @@
       <c r="R4" t="n">
         <v>6702.08531</v>
       </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
       <c r="U4" t="n">
         <v>6865.47324</v>
       </c>
@@ -902,21 +980,47 @@
       </c>
       <c r="AE4" t="n">
         <v>6039.3182152882</v>
+      </c>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>826.1550247118</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>6865.47324</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>54321 Total</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Study 1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
@@ -991,14 +1095,32 @@
       </c>
       <c r="AE5" t="n">
         <v>6045.923089093773</v>
+      </c>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>976.6129432291293</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>7022.536032322902</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
       <c r="D6" t="n">
         <v>65432</v>
       </c>
@@ -1012,10 +1134,18 @@
           <t>A</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
@@ -1040,8 +1170,12 @@
       <c r="R6" t="n">
         <v>42.60160124201722</v>
       </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
       <c r="U6" t="n">
         <v>180.0596631326561</v>
       </c>
@@ -1074,25 +1208,57 @@
       </c>
       <c r="AE6" t="n">
         <v>-111.226867427747</v>
+      </c>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>291.2865305604031</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>180.0596631326561</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>65432</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Study 2</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
@@ -1117,8 +1283,12 @@
       <c r="R7" t="n">
         <v>91.08320000000001</v>
       </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
       <c r="U7" t="n">
         <v>158.54728</v>
       </c>
@@ -1151,21 +1321,47 @@
       </c>
       <c r="AE7" t="n">
         <v>-1753.524880284128</v>
+      </c>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>1912.072160284128</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>158.54728</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>65432 Total</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Study 2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
@@ -1240,14 +1436,32 @@
       </c>
       <c r="AE8" t="n">
         <v>-1864.751747711875</v>
+      </c>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>2203.358690844531</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>338.6069431326561</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
       <c r="D9" t="n">
         <v>87653</v>
       </c>
@@ -1261,10 +1475,18 @@
           <t>A</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
@@ -1289,8 +1511,12 @@
       <c r="R9" t="n">
         <v>554.6238013340608</v>
       </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
       <c r="U9" t="n">
         <v>1085.326284925343</v>
       </c>
@@ -1323,21 +1549,47 @@
       </c>
       <c r="AE9" t="n">
         <v>-268.8825094126939</v>
+      </c>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>1354.208794338037</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>1085.326284925343</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Clinical</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>87653 Total</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Study 3</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
@@ -1412,21 +1664,47 @@
       </c>
       <c r="AE10" t="n">
         <v>-268.8825094126939</v>
+      </c>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>1354.208794338037</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>1085.326284925343</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>Clinical Total</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>87653 Total</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Study 3</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
@@ -1501,6 +1779,16 @@
       </c>
       <c r="AE11" t="n">
         <v>3912.288831969205</v>
+      </c>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>4534.180428411697</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>8446.469260380902</v>
       </c>
     </row>
     <row r="12">
@@ -1512,10 +1800,26 @@
           <t>Development Total</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Clinical Total</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>87653 Total</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Study 3</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
@@ -1590,6 +1894,16 @@
       </c>
       <c r="AE12" t="n">
         <v>3912.288831969205</v>
+      </c>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>4534.180428411697</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>8446.469260380902</v>
       </c>
     </row>
     <row r="13">
@@ -1601,10 +1915,26 @@
           <t>Grand Total</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Clinical Total</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>87653 Total</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Study 3</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
@@ -1680,6 +2010,198 @@
       <c r="AE13" t="n">
         <v>3912.288831969205</v>
       </c>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>4534.180428411697</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>8446.469260380902</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>recal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1417.598704893892</v>
+      </c>
+      <c r="M14" t="n">
+        <v>604.61526963542</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2226.315374733448</v>
+      </c>
+      <c r="O14" t="n">
+        <v>285.6510791489375</v>
+      </c>
+      <c r="P14" t="n">
+        <v>4534.180428411697</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>999.1874956821435</v>
+      </c>
+      <c r="R14" t="n">
+        <v>7447.281764698757</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>8446.469260380902</v>
+      </c>
+      <c r="V14" t="n">
+        <v>999.1874956821435</v>
+      </c>
+      <c r="W14" t="n">
+        <v>7447.281764698757</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>8446.469260380902</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>-418.4112092117485</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>6842.666495063337</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>-2226.315374733448</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>-285.6510791489375</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>3912.288831969205</v>
+      </c>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>variance</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Day8- working on the groupby function and the subtraction opr.
</commit_message>
<xml_diff>
--- a/new_book.xlsx
+++ b/new_book.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI15"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2024,89 +2024,48 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>recal</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>subtotal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0
+Budget Type            Variance FY 2021
+Development                11736.866496
+Development Total           3912.288832
+Grand Total                 3912.288832
+Name: Unnamed: 29, dtype: object</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1417.598704893892</v>
-      </c>
-      <c r="M14" t="n">
-        <v>604.61526963542</v>
-      </c>
-      <c r="N14" t="n">
-        <v>2226.315374733448</v>
-      </c>
-      <c r="O14" t="n">
-        <v>285.6510791489375</v>
-      </c>
-      <c r="P14" t="n">
-        <v>4534.180428411697</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>999.1874956821435</v>
-      </c>
-      <c r="R14" t="n">
-        <v>7447.281764698757</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" t="n">
-        <v>8446.469260380902</v>
-      </c>
-      <c r="V14" t="n">
-        <v>999.1874956821435</v>
-      </c>
-      <c r="W14" t="n">
-        <v>7447.281764698757</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>8446.469260380902</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>-418.4112092117485</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>6842.666495063337</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>-2226.315374733448</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>-285.6510791489375</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>3912.288831969205</v>
-      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr"/>
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
@@ -2115,7 +2074,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>variance</t>
+          <t>recal</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -2139,25 +2098,25 @@
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>1417.598704893892</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>604.61526963542</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>2226.315374733448</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>285.6510791489375</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>4534.180428411697</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>999.1874956821435</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>7447.281764698757</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -2166,13 +2125,13 @@
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
+        <v>8446.469260380902</v>
       </c>
       <c r="V15" t="n">
-        <v>0</v>
+        <v>999.1874956821435</v>
       </c>
       <c r="W15" t="n">
-        <v>0</v>
+        <v>7447.281764698757</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -2181,28 +2140,119 @@
         <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>8446.469260380902</v>
       </c>
       <c r="AA15" t="n">
-        <v>0</v>
+        <v>-418.4112092117485</v>
       </c>
       <c r="AB15" t="n">
-        <v>0</v>
+        <v>6842.666495063337</v>
       </c>
       <c r="AC15" t="n">
-        <v>0</v>
+        <v>-2226.315374733448</v>
       </c>
       <c r="AD15" t="n">
-        <v>0</v>
+        <v>-285.6510791489375</v>
       </c>
       <c r="AE15" t="n">
-        <v>0</v>
+        <v>3912.288831969205</v>
       </c>
       <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
     </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>variance</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Day8- update: able to export one column of groupby data to a new excel file. need to work on how to comb groupby result to a single dataframe and export.
</commit_message>
<xml_diff>
--- a/new_book.xlsx
+++ b/new_book.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI16"/>
+  <dimension ref="A1:AI15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2024,48 +2024,89 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>subtotal</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>0
-Budget Type            Variance FY 2021
-Development                11736.866496
-Development Total           3912.288832
-Grand Total                 3912.288832
-Name: Unnamed: 29, dtype: object</t>
-        </is>
-      </c>
+          <t>recal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1417.598704893892</v>
+      </c>
+      <c r="M14" t="n">
+        <v>604.61526963542</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2226.315374733448</v>
+      </c>
+      <c r="O14" t="n">
+        <v>285.6510791489375</v>
+      </c>
+      <c r="P14" t="n">
+        <v>4534.180428411697</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>999.1874956821435</v>
+      </c>
+      <c r="R14" t="n">
+        <v>7447.281764698757</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>8446.469260380902</v>
+      </c>
+      <c r="V14" t="n">
+        <v>999.1874956821435</v>
+      </c>
+      <c r="W14" t="n">
+        <v>7447.281764698757</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>8446.469260380902</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>-418.4112092117485</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>6842.666495063337</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>-2226.315374733448</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>-285.6510791489375</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>3912.288831969205</v>
+      </c>
       <c r="AF14" t="inlineStr"/>
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
@@ -2074,7 +2115,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>recal</t>
+          <t>variance</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -2098,25 +2139,25 @@
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>1417.598704893892</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>604.61526963542</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>2226.315374733448</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>285.6510791489375</v>
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>4534.180428411697</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>999.1874956821435</v>
+        <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>7447.281764698757</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -2125,13 +2166,13 @@
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>8446.469260380902</v>
+        <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>999.1874956821435</v>
+        <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>7447.281764698757</v>
+        <v>0</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -2140,119 +2181,28 @@
         <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>8446.469260380902</v>
+        <v>0</v>
       </c>
       <c r="AA15" t="n">
-        <v>-418.4112092117485</v>
+        <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>6842.666495063337</v>
+        <v>0</v>
       </c>
       <c r="AC15" t="n">
-        <v>-2226.315374733448</v>
+        <v>0</v>
       </c>
       <c r="AD15" t="n">
-        <v>-285.6510791489375</v>
+        <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>3912.288831969205</v>
+        <v>0</v>
       </c>
       <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>variance</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>0</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>